<commit_message>
Nach Aufteilung auf Hierachische Schaltpläne.
</commit_message>
<xml_diff>
--- a/range_calculation.xlsx
+++ b/range_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\voltagerecorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{442C62F6-25B9-42CF-AAC0-5482AB906AE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEC8416-8849-4738-96A0-96B7D9F724E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20690" yWindow="3860" windowWidth="14670" windowHeight="13760" xr2:uid="{7BF9E7E0-B672-44D9-A992-FF9B92BA5B15}"/>
+    <workbookView xWindow="15920" yWindow="3860" windowWidth="19700" windowHeight="13760" xr2:uid="{7BF9E7E0-B672-44D9-A992-FF9B92BA5B15}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>C / pF</t>
   </si>
@@ -67,12 +67,27 @@
   </si>
   <si>
     <t>Range Calculation</t>
+  </si>
+  <si>
+    <t>R / Ohm</t>
+  </si>
+  <si>
+    <t>C / nF</t>
+  </si>
+  <si>
+    <t>P / mW</t>
+  </si>
+  <si>
+    <t>U / V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -97,12 +112,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -117,11 +138,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -143,16 +167,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>673376</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>158951</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>590826</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>101801</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -175,7 +199,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3187700" y="361950"/>
+          <a:off x="3987800" y="2882900"/>
           <a:ext cx="5378726" cy="3911801"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -485,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94C54981-A60E-4B3E-BF37-6BF450D1D68D}">
-  <dimension ref="A3:C24"/>
+  <dimension ref="A3:C35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -512,7 +536,7 @@
         <v>1</v>
       </c>
       <c r="B8">
-        <v>390</v>
+        <v>470</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -520,7 +544,7 @@
         <v>2</v>
       </c>
       <c r="B9">
-        <v>390</v>
+        <v>470</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -528,7 +552,7 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
@@ -536,7 +560,7 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>8.1999999999999993</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -544,7 +568,7 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>120</v>
+        <v>150</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -564,11 +588,11 @@
       </c>
       <c r="B17" s="1">
         <f>(A17/$B$11)*($B$11+$B$10+$B$9+$B$8)</f>
-        <v>962.43902439024407</v>
+        <v>960</v>
       </c>
       <c r="C17" s="1">
         <f>B17/SQRT(2)</f>
-        <v>680.5471606249065</v>
+        <v>678.82250993908553</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -577,11 +601,11 @@
       </c>
       <c r="B18" s="1">
         <f t="shared" ref="B18:B19" si="0">(A18/$B$11)*($B$11+$B$10+$B$9+$B$8)</f>
-        <v>481.21951219512204</v>
+        <v>480</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" ref="C18:C19" si="1">B18/SQRT(2)</f>
-        <v>340.27358031245325</v>
+        <v>339.41125496954277</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -590,11 +614,11 @@
       </c>
       <c r="B19" s="1">
         <f t="shared" si="0"/>
-        <v>240.60975609756102</v>
+        <v>240</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="1"/>
-        <v>170.13679015622662</v>
+        <v>169.70562748477138</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -603,7 +627,71 @@
       </c>
       <c r="B24" s="1">
         <f>1/(2*PI()*(B11*(B8+B9+B10)/(B11+B10+B9+B8))*1000*B13*0.000000000001)*0.001</f>
-        <v>163.44102449450341</v>
+        <v>107.22017218822423</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1">
+        <f xml:space="preserve"> B27^2/SUM(B8:B11)</f>
+        <v>960</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>100</v>
+      </c>
+      <c r="B33">
+        <v>75</v>
+      </c>
+      <c r="C33" s="6">
+        <f>1/(2*PI()*B33*A33*1000)*1000000000</f>
+        <v>21.220659078919379</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>100</v>
+      </c>
+      <c r="B34" s="5">
+        <f>1/(2*PI()*A34*1000*C34*0.000000001)</f>
+        <v>106.10329539459687</v>
+      </c>
+      <c r="C34">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="5">
+        <f>1/(2*PI()*B35*C35*0.000000001)</f>
+        <v>117892.55043844097</v>
+      </c>
+      <c r="B35">
+        <v>75</v>
+      </c>
+      <c r="C35">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Schematic as pdf added.
</commit_message>
<xml_diff>
--- a/range_calculation.xlsx
+++ b/range_calculation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\voltagerecorder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GIT\voltagerecorder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FEC8416-8849-4738-96A0-96B7D9F724E8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7272EBD8-9D8B-4200-8CBE-C569093504A6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="3860" windowWidth="19700" windowHeight="13760" xr2:uid="{7BF9E7E0-B672-44D9-A992-FF9B92BA5B15}"/>
+    <workbookView xWindow="34785" yWindow="5490" windowWidth="17715" windowHeight="18945" xr2:uid="{7BF9E7E0-B672-44D9-A992-FF9B92BA5B15}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -512,26 +512,26 @@
   <dimension ref="A3:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.6328125" customWidth="1"/>
-    <col min="3" max="3" width="14.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:3" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -539,7 +539,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -547,7 +547,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -555,7 +555,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -563,7 +563,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -571,7 +571,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -582,7 +582,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -595,7 +595,7 @@
         <v>678.82250993908553</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5</v>
       </c>
@@ -608,7 +608,7 @@
         <v>339.41125496954277</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2.5</v>
       </c>
@@ -621,7 +621,7 @@
         <v>169.70562748477138</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -630,7 +630,7 @@
         <v>107.22017218822423</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>14</v>
       </c>
@@ -638,7 +638,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -647,7 +647,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>8</v>
       </c>
@@ -658,7 +658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>100</v>
       </c>
@@ -670,7 +670,7 @@
         <v>21.220659078919379</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>100</v>
       </c>
@@ -682,16 +682,16 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <f>1/(2*PI()*B35*C35*0.000000001)</f>
-        <v>117892.55043844097</v>
+        <v>106103.29539459689</v>
       </c>
       <c r="B35">
-        <v>75</v>
+        <v>100</v>
       </c>
       <c r="C35">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>